<commit_message>
Fix data and create folium map
</commit_message>
<xml_diff>
--- a/References/Jadual-2-3-sungai-tercemar-2020-geocoded.xlsx
+++ b/References/Jadual-2-3-sungai-tercemar-2020-geocoded.xlsx
@@ -1,13 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -558,16 +558,12 @@
           <t>Sg. Chempedak</t>
         </is>
       </c>
-      <c r="M2" t="inlineStr">
-        <is>
-          <t>Jalan Chempedak, Ang Mo Kio, Singapore, Central, 574416, Singapore</t>
-        </is>
-      </c>
+      <c r="M2" t="inlineStr"/>
       <c r="N2" t="n">
-        <v>1.3702991</v>
+        <v>5.2011951</v>
       </c>
       <c r="O2" t="n">
-        <v>103.829376</v>
+        <v>100.4944918</v>
       </c>
     </row>
     <row r="3">
@@ -688,16 +684,12 @@
           <t>Sg. Tengah</t>
         </is>
       </c>
-      <c r="M4" t="inlineStr">
-        <is>
-          <t>Tengah, Southwest, Singapore</t>
-        </is>
-      </c>
+      <c r="M4" t="inlineStr"/>
       <c r="N4" t="n">
-        <v>1.3655284</v>
+        <v>5.2011951</v>
       </c>
       <c r="O4" t="n">
-        <v>103.7307585</v>
+        <v>100.4944918</v>
       </c>
     </row>
     <row r="5">
@@ -2250,10 +2242,10 @@
         </is>
       </c>
       <c r="N28" t="n">
-        <v>-4.993518099999999</v>
+        <v>1.4888923</v>
       </c>
       <c r="O28" t="n">
-        <v>122.9519943371481</v>
+        <v>103.7957151</v>
       </c>
     </row>
     <row r="29">

</xml_diff>